<commit_message>
Crawler - Versão RC 3.0
</commit_message>
<xml_diff>
--- a/Crawler/noticias_final.xlsx
+++ b/Crawler/noticias_final.xlsx
@@ -16,9 +16,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="437">
   <si>
-    <t>Relevância</t>
-  </si>
-  <si>
     <t>João Doria e Márcio França participam de debate na TV; veja propostas</t>
   </si>
   <si>
@@ -1325,13 +1322,16 @@
   </si>
   <si>
     <t>LINK</t>
+  </si>
+  <si>
+    <t>Relevância2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1463,6 +1463,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1650,12 +1658,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1770,81 +1778,8 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1887,31 +1822,23 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Ênfase2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Ênfase3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1941,6 +1868,7 @@
     <cellStyle name="Ênfase5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Ênfase6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Hiperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Incorreto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutra" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1955,7 +1883,11 @@
     <cellStyle name="Título 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1963,6 +1895,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:D225" totalsRowShown="0">
+  <autoFilter ref="A1:D225"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="RELEVÂNCIA" dataDxfId="0"/>
+    <tableColumn id="2" name="TÍTULO DA NOTÍCIA"/>
+    <tableColumn id="3" name="LINK"/>
+    <tableColumn id="4" name="Relevância2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2255,39 +2200,40 @@
   <dimension ref="A1:D225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="122.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" t="s">
         <v>436</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>1</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2298,10 +2244,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -2312,10 +2258,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2326,10 +2272,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2340,10 +2286,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -2354,10 +2300,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -2368,10 +2314,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2382,10 +2328,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -2396,10 +2342,10 @@
         <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -2410,10 +2356,10 @@
         <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -2424,10 +2370,10 @@
         <v>1</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -2438,10 +2384,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -2452,10 +2398,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -2466,10 +2412,10 @@
         <v>1</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -2480,10 +2426,10 @@
         <v>1</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -2494,10 +2440,10 @@
         <v>1</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -2508,10 +2454,10 @@
         <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -2522,10 +2468,10 @@
         <v>1</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -2536,10 +2482,10 @@
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -2550,10 +2496,10 @@
         <v>1</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -2564,10 +2510,10 @@
         <v>1</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -2578,10 +2524,10 @@
         <v>1</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -2592,10 +2538,10 @@
         <v>1</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -2606,10 +2552,10 @@
         <v>1</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -2620,10 +2566,10 @@
         <v>1</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -2634,10 +2580,10 @@
         <v>1</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -2648,10 +2594,10 @@
         <v>1</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -2662,10 +2608,10 @@
         <v>1</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -2676,10 +2622,10 @@
         <v>1</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -2690,10 +2636,10 @@
         <v>1</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -2704,10 +2650,10 @@
         <v>1</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -2718,10 +2664,10 @@
         <v>1</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -2732,10 +2678,10 @@
         <v>1</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -2746,10 +2692,10 @@
         <v>1</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -2760,10 +2706,10 @@
         <v>1</v>
       </c>
       <c r="B36" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -2774,10 +2720,10 @@
         <v>1</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -2788,10 +2734,10 @@
         <v>1</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -2802,10 +2748,10 @@
         <v>1</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -2816,10 +2762,10 @@
         <v>1</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -2830,10 +2776,10 @@
         <v>1</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -2844,10 +2790,10 @@
         <v>1</v>
       </c>
       <c r="B42" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -2858,10 +2804,10 @@
         <v>1</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -2872,10 +2818,10 @@
         <v>1</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -2886,10 +2832,10 @@
         <v>1</v>
       </c>
       <c r="B45" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -2900,10 +2846,10 @@
         <v>1</v>
       </c>
       <c r="B46" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -2914,10 +2860,10 @@
         <v>1</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -2928,10 +2874,10 @@
         <v>1</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -2942,10 +2888,10 @@
         <v>1</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -2956,10 +2902,10 @@
         <v>1</v>
       </c>
       <c r="B50" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -2970,10 +2916,10 @@
         <v>1</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -2984,10 +2930,10 @@
         <v>1</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -2998,10 +2944,10 @@
         <v>1</v>
       </c>
       <c r="B53" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -3012,10 +2958,10 @@
         <v>1</v>
       </c>
       <c r="B54" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D54">
         <v>1</v>
@@ -3026,10 +2972,10 @@
         <v>1</v>
       </c>
       <c r="B55" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -3040,10 +2986,10 @@
         <v>1</v>
       </c>
       <c r="B56" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -3054,10 +3000,10 @@
         <v>2</v>
       </c>
       <c r="B57" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="D57">
         <v>2</v>
@@ -3068,10 +3014,10 @@
         <v>2</v>
       </c>
       <c r="B58" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C58" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="D58">
         <v>2</v>
@@ -3082,10 +3028,10 @@
         <v>2</v>
       </c>
       <c r="B59" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C59" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="D59">
         <v>2</v>
@@ -3096,10 +3042,10 @@
         <v>2</v>
       </c>
       <c r="B60" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C60" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="D60">
         <v>2</v>
@@ -3110,10 +3056,10 @@
         <v>2</v>
       </c>
       <c r="B61" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>119</v>
       </c>
       <c r="D61">
         <v>2</v>
@@ -3124,10 +3070,10 @@
         <v>2</v>
       </c>
       <c r="B62" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C62" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>121</v>
       </c>
       <c r="D62">
         <v>2</v>
@@ -3138,10 +3084,10 @@
         <v>2</v>
       </c>
       <c r="B63" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="D63">
         <v>2</v>
@@ -3152,10 +3098,10 @@
         <v>2</v>
       </c>
       <c r="B64" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C64" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>125</v>
       </c>
       <c r="D64">
         <v>2</v>
@@ -3166,10 +3112,10 @@
         <v>2</v>
       </c>
       <c r="B65" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>127</v>
       </c>
       <c r="D65">
         <v>2</v>
@@ -3180,10 +3126,10 @@
         <v>2</v>
       </c>
       <c r="B66" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C66" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>129</v>
       </c>
       <c r="D66">
         <v>2</v>
@@ -3194,10 +3140,10 @@
         <v>2</v>
       </c>
       <c r="B67" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C67" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="D67">
         <v>2</v>
@@ -3208,10 +3154,10 @@
         <v>2</v>
       </c>
       <c r="B68" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C68" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>133</v>
       </c>
       <c r="D68">
         <v>2</v>
@@ -3222,10 +3168,10 @@
         <v>2</v>
       </c>
       <c r="B69" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>135</v>
       </c>
       <c r="D69">
         <v>2</v>
@@ -3236,10 +3182,10 @@
         <v>2</v>
       </c>
       <c r="B70" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>137</v>
       </c>
       <c r="D70">
         <v>2</v>
@@ -3250,10 +3196,10 @@
         <v>2</v>
       </c>
       <c r="B71" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C71" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>139</v>
       </c>
       <c r="D71">
         <v>2</v>
@@ -3264,10 +3210,10 @@
         <v>2</v>
       </c>
       <c r="B72" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C72" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="D72">
         <v>2</v>
@@ -3278,10 +3224,10 @@
         <v>2</v>
       </c>
       <c r="B73" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C73" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>143</v>
       </c>
       <c r="D73">
         <v>2</v>
@@ -3292,10 +3238,10 @@
         <v>2</v>
       </c>
       <c r="B74" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C74" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>145</v>
       </c>
       <c r="D74">
         <v>2</v>
@@ -3306,10 +3252,10 @@
         <v>2</v>
       </c>
       <c r="B75" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C75" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>147</v>
       </c>
       <c r="D75">
         <v>2</v>
@@ -3320,10 +3266,10 @@
         <v>2</v>
       </c>
       <c r="B76" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C76" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>149</v>
       </c>
       <c r="D76">
         <v>2</v>
@@ -3334,10 +3280,10 @@
         <v>2</v>
       </c>
       <c r="B77" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C77" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>151</v>
       </c>
       <c r="D77">
         <v>2</v>
@@ -3348,10 +3294,10 @@
         <v>2</v>
       </c>
       <c r="B78" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C78" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>153</v>
       </c>
       <c r="D78">
         <v>2</v>
@@ -3362,10 +3308,10 @@
         <v>2</v>
       </c>
       <c r="B79" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C79" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>155</v>
       </c>
       <c r="D79">
         <v>2</v>
@@ -3376,10 +3322,10 @@
         <v>2</v>
       </c>
       <c r="B80" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C80" s="3" t="s">
         <v>156</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>157</v>
       </c>
       <c r="D80">
         <v>2</v>
@@ -3390,10 +3336,10 @@
         <v>2</v>
       </c>
       <c r="B81" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C81" s="3" t="s">
         <v>158</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>159</v>
       </c>
       <c r="D81">
         <v>2</v>
@@ -3404,10 +3350,10 @@
         <v>2</v>
       </c>
       <c r="B82" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C82" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>161</v>
       </c>
       <c r="D82">
         <v>2</v>
@@ -3418,10 +3364,10 @@
         <v>2</v>
       </c>
       <c r="B83" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C83" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D83">
         <v>2</v>
@@ -3432,10 +3378,10 @@
         <v>2</v>
       </c>
       <c r="B84" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C84" s="3" t="s">
         <v>164</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>165</v>
       </c>
       <c r="D84">
         <v>2</v>
@@ -3446,10 +3392,10 @@
         <v>2</v>
       </c>
       <c r="B85" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C85" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>167</v>
       </c>
       <c r="D85">
         <v>2</v>
@@ -3460,10 +3406,10 @@
         <v>2</v>
       </c>
       <c r="B86" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C86" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>169</v>
       </c>
       <c r="D86">
         <v>2</v>
@@ -3474,10 +3420,10 @@
         <v>2</v>
       </c>
       <c r="B87" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C87" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>171</v>
       </c>
       <c r="D87">
         <v>2</v>
@@ -3488,10 +3434,10 @@
         <v>2</v>
       </c>
       <c r="B88" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C88" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>173</v>
       </c>
       <c r="D88">
         <v>2</v>
@@ -3502,10 +3448,10 @@
         <v>2</v>
       </c>
       <c r="B89" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C89" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>175</v>
       </c>
       <c r="D89">
         <v>2</v>
@@ -3516,10 +3462,10 @@
         <v>2</v>
       </c>
       <c r="B90" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C90" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>177</v>
       </c>
       <c r="D90">
         <v>2</v>
@@ -3530,10 +3476,10 @@
         <v>2</v>
       </c>
       <c r="B91" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C91" s="3" t="s">
         <v>178</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>179</v>
       </c>
       <c r="D91">
         <v>2</v>
@@ -3544,10 +3490,10 @@
         <v>2</v>
       </c>
       <c r="B92" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C92" s="3" t="s">
         <v>180</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>181</v>
       </c>
       <c r="D92">
         <v>2</v>
@@ -3558,10 +3504,10 @@
         <v>2</v>
       </c>
       <c r="B93" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C93" s="3" t="s">
         <v>182</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>183</v>
       </c>
       <c r="D93">
         <v>2</v>
@@ -3572,10 +3518,10 @@
         <v>2</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D94">
         <v>2</v>
@@ -3586,10 +3532,10 @@
         <v>2</v>
       </c>
       <c r="B95" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C95" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>186</v>
       </c>
       <c r="D95">
         <v>2</v>
@@ -3600,10 +3546,10 @@
         <v>2</v>
       </c>
       <c r="B96" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C96" s="3" t="s">
         <v>187</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>188</v>
       </c>
       <c r="D96">
         <v>2</v>
@@ -3614,10 +3560,10 @@
         <v>2</v>
       </c>
       <c r="B97" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C97" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>190</v>
       </c>
       <c r="D97">
         <v>2</v>
@@ -3628,10 +3574,10 @@
         <v>2</v>
       </c>
       <c r="B98" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C98" s="3" t="s">
         <v>191</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>192</v>
       </c>
       <c r="D98">
         <v>2</v>
@@ -3642,10 +3588,10 @@
         <v>2</v>
       </c>
       <c r="B99" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C99" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>194</v>
       </c>
       <c r="D99">
         <v>2</v>
@@ -3656,10 +3602,10 @@
         <v>2</v>
       </c>
       <c r="B100" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C100" s="3" t="s">
         <v>195</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>196</v>
       </c>
       <c r="D100">
         <v>2</v>
@@ -3670,10 +3616,10 @@
         <v>3</v>
       </c>
       <c r="B101" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C101" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>198</v>
       </c>
       <c r="D101">
         <v>3</v>
@@ -3684,10 +3630,10 @@
         <v>3</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D102">
         <v>3</v>
@@ -3698,10 +3644,10 @@
         <v>3</v>
       </c>
       <c r="B103" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C103" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>201</v>
       </c>
       <c r="D103">
         <v>3</v>
@@ -3712,10 +3658,10 @@
         <v>3</v>
       </c>
       <c r="B104" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C104" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>203</v>
       </c>
       <c r="D104">
         <v>3</v>
@@ -3726,10 +3672,10 @@
         <v>3</v>
       </c>
       <c r="B105" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C105" s="3" t="s">
         <v>204</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>205</v>
       </c>
       <c r="D105">
         <v>3</v>
@@ -3740,10 +3686,10 @@
         <v>3</v>
       </c>
       <c r="B106" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C106" s="3" t="s">
         <v>206</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>207</v>
       </c>
       <c r="D106">
         <v>3</v>
@@ -3754,10 +3700,10 @@
         <v>3</v>
       </c>
       <c r="B107" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C107" s="3" t="s">
         <v>208</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>209</v>
       </c>
       <c r="D107">
         <v>3</v>
@@ -3768,10 +3714,10 @@
         <v>3</v>
       </c>
       <c r="B108" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C108" s="3" t="s">
         <v>210</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>211</v>
       </c>
       <c r="D108">
         <v>3</v>
@@ -3782,10 +3728,10 @@
         <v>3</v>
       </c>
       <c r="B109" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C109" s="3" t="s">
         <v>212</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>213</v>
       </c>
       <c r="D109">
         <v>3</v>
@@ -3796,10 +3742,10 @@
         <v>3</v>
       </c>
       <c r="B110" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C110" s="3" t="s">
         <v>214</v>
-      </c>
-      <c r="C110" s="3" t="s">
-        <v>215</v>
       </c>
       <c r="D110">
         <v>3</v>
@@ -3810,10 +3756,10 @@
         <v>3</v>
       </c>
       <c r="B111" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C111" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>217</v>
       </c>
       <c r="D111">
         <v>3</v>
@@ -3824,10 +3770,10 @@
         <v>3</v>
       </c>
       <c r="B112" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C112" s="3" t="s">
         <v>218</v>
-      </c>
-      <c r="C112" s="3" t="s">
-        <v>219</v>
       </c>
       <c r="D112">
         <v>3</v>
@@ -3838,10 +3784,10 @@
         <v>3</v>
       </c>
       <c r="B113" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C113" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>221</v>
       </c>
       <c r="D113">
         <v>3</v>
@@ -3852,10 +3798,10 @@
         <v>3</v>
       </c>
       <c r="B114" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C114" s="3" t="s">
         <v>222</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>223</v>
       </c>
       <c r="D114">
         <v>3</v>
@@ -3866,10 +3812,10 @@
         <v>3</v>
       </c>
       <c r="B115" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C115" s="3" t="s">
         <v>224</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>225</v>
       </c>
       <c r="D115">
         <v>3</v>
@@ -3880,10 +3826,10 @@
         <v>3</v>
       </c>
       <c r="B116" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C116" s="3" t="s">
         <v>226</v>
-      </c>
-      <c r="C116" s="3" t="s">
-        <v>227</v>
       </c>
       <c r="D116">
         <v>3</v>
@@ -3894,10 +3840,10 @@
         <v>3</v>
       </c>
       <c r="B117" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C117" s="3" t="s">
         <v>228</v>
-      </c>
-      <c r="C117" s="3" t="s">
-        <v>229</v>
       </c>
       <c r="D117">
         <v>3</v>
@@ -3908,10 +3854,10 @@
         <v>3</v>
       </c>
       <c r="B118" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C118" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="C118" s="3" t="s">
-        <v>231</v>
       </c>
       <c r="D118">
         <v>3</v>
@@ -3922,10 +3868,10 @@
         <v>3</v>
       </c>
       <c r="B119" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C119" s="3" t="s">
         <v>232</v>
-      </c>
-      <c r="C119" s="3" t="s">
-        <v>233</v>
       </c>
       <c r="D119">
         <v>3</v>
@@ -3936,10 +3882,10 @@
         <v>3</v>
       </c>
       <c r="B120" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C120" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="C120" s="3" t="s">
-        <v>235</v>
       </c>
       <c r="D120">
         <v>3</v>
@@ -3950,10 +3896,10 @@
         <v>3</v>
       </c>
       <c r="B121" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C121" s="3" t="s">
         <v>236</v>
-      </c>
-      <c r="C121" s="3" t="s">
-        <v>237</v>
       </c>
       <c r="D121">
         <v>3</v>
@@ -3964,10 +3910,10 @@
         <v>3</v>
       </c>
       <c r="B122" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C122" s="3" t="s">
         <v>238</v>
-      </c>
-      <c r="C122" s="3" t="s">
-        <v>239</v>
       </c>
       <c r="D122">
         <v>3</v>
@@ -3978,10 +3924,10 @@
         <v>3</v>
       </c>
       <c r="B123" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C123" s="3" t="s">
         <v>240</v>
-      </c>
-      <c r="C123" s="3" t="s">
-        <v>241</v>
       </c>
       <c r="D123">
         <v>3</v>
@@ -3992,10 +3938,10 @@
         <v>3</v>
       </c>
       <c r="B124" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C124" s="3" t="s">
         <v>242</v>
-      </c>
-      <c r="C124" s="3" t="s">
-        <v>243</v>
       </c>
       <c r="D124">
         <v>3</v>
@@ -4006,10 +3952,10 @@
         <v>3</v>
       </c>
       <c r="B125" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C125" s="3" t="s">
         <v>244</v>
-      </c>
-      <c r="C125" s="3" t="s">
-        <v>245</v>
       </c>
       <c r="D125">
         <v>3</v>
@@ -4020,10 +3966,10 @@
         <v>3</v>
       </c>
       <c r="B126" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C126" s="3" t="s">
         <v>246</v>
-      </c>
-      <c r="C126" s="3" t="s">
-        <v>247</v>
       </c>
       <c r="D126">
         <v>3</v>
@@ -4034,10 +3980,10 @@
         <v>3</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D127">
         <v>3</v>
@@ -4048,10 +3994,10 @@
         <v>3</v>
       </c>
       <c r="B128" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C128" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="C128" s="3" t="s">
-        <v>250</v>
       </c>
       <c r="D128">
         <v>3</v>
@@ -4062,10 +4008,10 @@
         <v>3</v>
       </c>
       <c r="B129" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="C129" s="3" t="s">
         <v>251</v>
-      </c>
-      <c r="C129" s="3" t="s">
-        <v>252</v>
       </c>
       <c r="D129">
         <v>3</v>
@@ -4076,10 +4022,10 @@
         <v>3</v>
       </c>
       <c r="B130" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C130" s="3" t="s">
         <v>253</v>
-      </c>
-      <c r="C130" s="3" t="s">
-        <v>254</v>
       </c>
       <c r="D130">
         <v>3</v>
@@ -4090,10 +4036,10 @@
         <v>3</v>
       </c>
       <c r="B131" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C131" s="3" t="s">
         <v>255</v>
-      </c>
-      <c r="C131" s="3" t="s">
-        <v>256</v>
       </c>
       <c r="D131">
         <v>3</v>
@@ -4104,10 +4050,10 @@
         <v>3</v>
       </c>
       <c r="B132" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="C132" s="3" t="s">
         <v>257</v>
-      </c>
-      <c r="C132" s="3" t="s">
-        <v>258</v>
       </c>
       <c r="D132">
         <v>3</v>
@@ -4118,10 +4064,10 @@
         <v>3</v>
       </c>
       <c r="B133" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C133" s="3" t="s">
         <v>259</v>
-      </c>
-      <c r="C133" s="3" t="s">
-        <v>260</v>
       </c>
       <c r="D133">
         <v>3</v>
@@ -4132,10 +4078,10 @@
         <v>3</v>
       </c>
       <c r="B134" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C134" s="3" t="s">
         <v>261</v>
-      </c>
-      <c r="C134" s="3" t="s">
-        <v>262</v>
       </c>
       <c r="D134">
         <v>3</v>
@@ -4146,10 +4092,10 @@
         <v>3</v>
       </c>
       <c r="B135" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="C135" s="3" t="s">
         <v>263</v>
-      </c>
-      <c r="C135" s="3" t="s">
-        <v>264</v>
       </c>
       <c r="D135">
         <v>3</v>
@@ -4160,10 +4106,10 @@
         <v>4</v>
       </c>
       <c r="B136" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C136" s="3" t="s">
         <v>265</v>
-      </c>
-      <c r="C136" s="3" t="s">
-        <v>266</v>
       </c>
       <c r="D136">
         <v>4</v>
@@ -4174,10 +4120,10 @@
         <v>4</v>
       </c>
       <c r="B137" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C137" s="3" t="s">
         <v>267</v>
-      </c>
-      <c r="C137" s="3" t="s">
-        <v>268</v>
       </c>
       <c r="D137">
         <v>4</v>
@@ -4188,10 +4134,10 @@
         <v>4</v>
       </c>
       <c r="B138" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C138" s="3" t="s">
         <v>269</v>
-      </c>
-      <c r="C138" s="3" t="s">
-        <v>270</v>
       </c>
       <c r="D138">
         <v>4</v>
@@ -4202,10 +4148,10 @@
         <v>4</v>
       </c>
       <c r="B139" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C139" s="3" t="s">
         <v>271</v>
-      </c>
-      <c r="C139" s="3" t="s">
-        <v>272</v>
       </c>
       <c r="D139">
         <v>4</v>
@@ -4216,10 +4162,10 @@
         <v>4</v>
       </c>
       <c r="B140" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="C140" s="3" t="s">
         <v>273</v>
-      </c>
-      <c r="C140" s="3" t="s">
-        <v>274</v>
       </c>
       <c r="D140">
         <v>4</v>
@@ -4230,10 +4176,10 @@
         <v>4</v>
       </c>
       <c r="B141" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C141" s="3" t="s">
         <v>275</v>
-      </c>
-      <c r="C141" s="3" t="s">
-        <v>276</v>
       </c>
       <c r="D141">
         <v>4</v>
@@ -4244,10 +4190,10 @@
         <v>4</v>
       </c>
       <c r="B142" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C142" s="3" t="s">
         <v>277</v>
-      </c>
-      <c r="C142" s="3" t="s">
-        <v>278</v>
       </c>
       <c r="D142">
         <v>4</v>
@@ -4258,10 +4204,10 @@
         <v>4</v>
       </c>
       <c r="B143" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C143" s="3" t="s">
         <v>279</v>
-      </c>
-      <c r="C143" s="3" t="s">
-        <v>280</v>
       </c>
       <c r="D143">
         <v>4</v>
@@ -4272,10 +4218,10 @@
         <v>4</v>
       </c>
       <c r="B144" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C144" s="3" t="s">
         <v>281</v>
-      </c>
-      <c r="C144" s="3" t="s">
-        <v>282</v>
       </c>
       <c r="D144">
         <v>4</v>
@@ -4286,10 +4232,10 @@
         <v>4</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D145">
         <v>4</v>
@@ -4300,10 +4246,10 @@
         <v>4</v>
       </c>
       <c r="B146" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C146" s="3" t="s">
         <v>284</v>
-      </c>
-      <c r="C146" s="3" t="s">
-        <v>285</v>
       </c>
       <c r="D146">
         <v>4</v>
@@ -4314,10 +4260,10 @@
         <v>4</v>
       </c>
       <c r="B147" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C147" s="3" t="s">
         <v>286</v>
-      </c>
-      <c r="C147" s="3" t="s">
-        <v>287</v>
       </c>
       <c r="D147">
         <v>4</v>
@@ -4328,10 +4274,10 @@
         <v>4</v>
       </c>
       <c r="B148" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C148" s="3" t="s">
         <v>288</v>
-      </c>
-      <c r="C148" s="3" t="s">
-        <v>289</v>
       </c>
       <c r="D148">
         <v>4</v>
@@ -4342,10 +4288,10 @@
         <v>4</v>
       </c>
       <c r="B149" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="C149" s="3" t="s">
         <v>290</v>
-      </c>
-      <c r="C149" s="3" t="s">
-        <v>291</v>
       </c>
       <c r="D149">
         <v>4</v>
@@ -4356,10 +4302,10 @@
         <v>4</v>
       </c>
       <c r="B150" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="C150" s="3" t="s">
         <v>292</v>
-      </c>
-      <c r="C150" s="3" t="s">
-        <v>293</v>
       </c>
       <c r="D150">
         <v>4</v>
@@ -4370,10 +4316,10 @@
         <v>4</v>
       </c>
       <c r="B151" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="C151" s="3" t="s">
         <v>294</v>
-      </c>
-      <c r="C151" s="3" t="s">
-        <v>295</v>
       </c>
       <c r="D151">
         <v>4</v>
@@ -4384,10 +4330,10 @@
         <v>4</v>
       </c>
       <c r="B152" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="C152" s="3" t="s">
         <v>296</v>
-      </c>
-      <c r="C152" s="3" t="s">
-        <v>297</v>
       </c>
       <c r="D152">
         <v>4</v>
@@ -4398,10 +4344,10 @@
         <v>4</v>
       </c>
       <c r="B153" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C153" s="3" t="s">
         <v>298</v>
-      </c>
-      <c r="C153" s="3" t="s">
-        <v>299</v>
       </c>
       <c r="D153">
         <v>4</v>
@@ -4412,10 +4358,10 @@
         <v>4</v>
       </c>
       <c r="B154" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="C154" s="3" t="s">
         <v>300</v>
-      </c>
-      <c r="C154" s="3" t="s">
-        <v>301</v>
       </c>
       <c r="D154">
         <v>4</v>
@@ -4426,10 +4372,10 @@
         <v>4</v>
       </c>
       <c r="B155" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="C155" s="3" t="s">
         <v>302</v>
-      </c>
-      <c r="C155" s="3" t="s">
-        <v>303</v>
       </c>
       <c r="D155">
         <v>4</v>
@@ -4440,10 +4386,10 @@
         <v>4</v>
       </c>
       <c r="B156" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="C156" s="3" t="s">
         <v>304</v>
-      </c>
-      <c r="C156" s="3" t="s">
-        <v>305</v>
       </c>
       <c r="D156">
         <v>4</v>
@@ -4454,10 +4400,10 @@
         <v>4</v>
       </c>
       <c r="B157" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="C157" s="3" t="s">
         <v>306</v>
-      </c>
-      <c r="C157" s="3" t="s">
-        <v>307</v>
       </c>
       <c r="D157">
         <v>4</v>
@@ -4468,10 +4414,10 @@
         <v>4</v>
       </c>
       <c r="B158" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="C158" s="3" t="s">
         <v>308</v>
-      </c>
-      <c r="C158" s="3" t="s">
-        <v>309</v>
       </c>
       <c r="D158">
         <v>4</v>
@@ -4482,10 +4428,10 @@
         <v>4</v>
       </c>
       <c r="B159" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C159" s="3" t="s">
         <v>310</v>
-      </c>
-      <c r="C159" s="3" t="s">
-        <v>311</v>
       </c>
       <c r="D159">
         <v>4</v>
@@ -4496,10 +4442,10 @@
         <v>4</v>
       </c>
       <c r="B160" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C160" s="3" t="s">
         <v>312</v>
-      </c>
-      <c r="C160" s="3" t="s">
-        <v>313</v>
       </c>
       <c r="D160">
         <v>4</v>
@@ -4510,10 +4456,10 @@
         <v>4</v>
       </c>
       <c r="B161" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C161" s="3" t="s">
         <v>314</v>
-      </c>
-      <c r="C161" s="3" t="s">
-        <v>315</v>
       </c>
       <c r="D161">
         <v>4</v>
@@ -4524,10 +4470,10 @@
         <v>4</v>
       </c>
       <c r="B162" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C162" s="3" t="s">
         <v>316</v>
-      </c>
-      <c r="C162" s="3" t="s">
-        <v>317</v>
       </c>
       <c r="D162">
         <v>4</v>
@@ -4538,10 +4484,10 @@
         <v>4</v>
       </c>
       <c r="B163" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="C163" s="3" t="s">
         <v>318</v>
-      </c>
-      <c r="C163" s="3" t="s">
-        <v>319</v>
       </c>
       <c r="D163">
         <v>4</v>
@@ -4552,10 +4498,10 @@
         <v>4</v>
       </c>
       <c r="B164" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="C164" s="3" t="s">
         <v>320</v>
-      </c>
-      <c r="C164" s="3" t="s">
-        <v>321</v>
       </c>
       <c r="D164">
         <v>4</v>
@@ -4566,10 +4512,10 @@
         <v>4</v>
       </c>
       <c r="B165" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C165" s="3" t="s">
         <v>322</v>
-      </c>
-      <c r="C165" s="3" t="s">
-        <v>323</v>
       </c>
       <c r="D165">
         <v>4</v>
@@ -4580,10 +4526,10 @@
         <v>4</v>
       </c>
       <c r="B166" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C166" s="3" t="s">
         <v>324</v>
-      </c>
-      <c r="C166" s="3" t="s">
-        <v>325</v>
       </c>
       <c r="D166">
         <v>4</v>
@@ -4594,10 +4540,10 @@
         <v>4</v>
       </c>
       <c r="B167" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C167" s="3" t="s">
         <v>326</v>
-      </c>
-      <c r="C167" s="3" t="s">
-        <v>327</v>
       </c>
       <c r="D167">
         <v>4</v>
@@ -4608,10 +4554,10 @@
         <v>4</v>
       </c>
       <c r="B168" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C168" s="3" t="s">
         <v>328</v>
-      </c>
-      <c r="C168" s="3" t="s">
-        <v>329</v>
       </c>
       <c r="D168">
         <v>4</v>
@@ -4622,10 +4568,10 @@
         <v>4</v>
       </c>
       <c r="B169" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C169" s="3" t="s">
         <v>330</v>
-      </c>
-      <c r="C169" s="3" t="s">
-        <v>331</v>
       </c>
       <c r="D169">
         <v>4</v>
@@ -4636,10 +4582,10 @@
         <v>5</v>
       </c>
       <c r="B170" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C170" s="3" t="s">
         <v>332</v>
-      </c>
-      <c r="C170" s="3" t="s">
-        <v>333</v>
       </c>
       <c r="D170">
         <v>5</v>
@@ -4650,10 +4596,10 @@
         <v>5</v>
       </c>
       <c r="B171" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="C171" s="3" t="s">
         <v>334</v>
-      </c>
-      <c r="C171" s="3" t="s">
-        <v>335</v>
       </c>
       <c r="D171">
         <v>5</v>
@@ -4664,10 +4610,10 @@
         <v>5</v>
       </c>
       <c r="B172" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="C172" s="3" t="s">
         <v>336</v>
-      </c>
-      <c r="C172" s="3" t="s">
-        <v>337</v>
       </c>
       <c r="D172">
         <v>5</v>
@@ -4678,10 +4624,10 @@
         <v>5</v>
       </c>
       <c r="B173" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="C173" s="3" t="s">
         <v>338</v>
-      </c>
-      <c r="C173" s="3" t="s">
-        <v>339</v>
       </c>
       <c r="D173">
         <v>5</v>
@@ -4692,10 +4638,10 @@
         <v>5</v>
       </c>
       <c r="B174" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="C174" s="3" t="s">
         <v>340</v>
-      </c>
-      <c r="C174" s="3" t="s">
-        <v>341</v>
       </c>
       <c r="D174">
         <v>5</v>
@@ -4706,10 +4652,10 @@
         <v>5</v>
       </c>
       <c r="B175" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="C175" s="3" t="s">
         <v>342</v>
-      </c>
-      <c r="C175" s="3" t="s">
-        <v>343</v>
       </c>
       <c r="D175">
         <v>5</v>
@@ -4720,10 +4666,10 @@
         <v>5</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D176">
         <v>5</v>
@@ -4734,10 +4680,10 @@
         <v>5</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D177">
         <v>5</v>
@@ -4748,10 +4694,10 @@
         <v>5</v>
       </c>
       <c r="B178" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="C178" s="3" t="s">
         <v>346</v>
-      </c>
-      <c r="C178" s="3" t="s">
-        <v>347</v>
       </c>
       <c r="D178">
         <v>5</v>
@@ -4762,10 +4708,10 @@
         <v>5</v>
       </c>
       <c r="B179" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="C179" s="3" t="s">
         <v>348</v>
-      </c>
-      <c r="C179" s="3" t="s">
-        <v>349</v>
       </c>
       <c r="D179">
         <v>5</v>
@@ -4776,10 +4722,10 @@
         <v>5</v>
       </c>
       <c r="B180" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="C180" s="3" t="s">
         <v>350</v>
-      </c>
-      <c r="C180" s="3" t="s">
-        <v>351</v>
       </c>
       <c r="D180">
         <v>5</v>
@@ -4790,10 +4736,10 @@
         <v>5</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D181">
         <v>5</v>
@@ -4804,10 +4750,10 @@
         <v>5</v>
       </c>
       <c r="B182" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C182" s="3" t="s">
         <v>353</v>
-      </c>
-      <c r="C182" s="3" t="s">
-        <v>354</v>
       </c>
       <c r="D182">
         <v>5</v>
@@ -4818,10 +4764,10 @@
         <v>5</v>
       </c>
       <c r="B183" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="C183" s="3" t="s">
         <v>355</v>
-      </c>
-      <c r="C183" s="3" t="s">
-        <v>356</v>
       </c>
       <c r="D183">
         <v>5</v>
@@ -4832,10 +4778,10 @@
         <v>5</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C184" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D184">
         <v>5</v>
@@ -4846,10 +4792,10 @@
         <v>5</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C185" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D185">
         <v>5</v>
@@ -4860,10 +4806,10 @@
         <v>5</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C186" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D186">
         <v>5</v>
@@ -4874,10 +4820,10 @@
         <v>5</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D187">
         <v>5</v>
@@ -4888,10 +4834,10 @@
         <v>5</v>
       </c>
       <c r="B188" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C188" s="3" t="s">
         <v>361</v>
-      </c>
-      <c r="C188" s="3" t="s">
-        <v>362</v>
       </c>
       <c r="D188">
         <v>5</v>
@@ -4902,10 +4848,10 @@
         <v>5</v>
       </c>
       <c r="B189" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="C189" s="3" t="s">
         <v>363</v>
-      </c>
-      <c r="C189" s="3" t="s">
-        <v>364</v>
       </c>
       <c r="D189">
         <v>5</v>
@@ -4916,10 +4862,10 @@
         <v>5</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D190">
         <v>5</v>
@@ -4930,10 +4876,10 @@
         <v>5</v>
       </c>
       <c r="B191" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="C191" s="3" t="s">
         <v>366</v>
-      </c>
-      <c r="C191" s="3" t="s">
-        <v>367</v>
       </c>
       <c r="D191">
         <v>5</v>
@@ -4944,10 +4890,10 @@
         <v>5</v>
       </c>
       <c r="B192" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="C192" s="3" t="s">
         <v>368</v>
-      </c>
-      <c r="C192" s="3" t="s">
-        <v>369</v>
       </c>
       <c r="D192">
         <v>5</v>
@@ -4958,10 +4904,10 @@
         <v>5</v>
       </c>
       <c r="B193" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="C193" s="3" t="s">
         <v>370</v>
-      </c>
-      <c r="C193" s="3" t="s">
-        <v>371</v>
       </c>
       <c r="D193">
         <v>5</v>
@@ -4972,10 +4918,10 @@
         <v>5</v>
       </c>
       <c r="B194" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="C194" s="3" t="s">
         <v>372</v>
-      </c>
-      <c r="C194" s="3" t="s">
-        <v>373</v>
       </c>
       <c r="D194">
         <v>5</v>
@@ -4986,10 +4932,10 @@
         <v>5</v>
       </c>
       <c r="B195" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="C195" s="3" t="s">
         <v>374</v>
-      </c>
-      <c r="C195" s="3" t="s">
-        <v>375</v>
       </c>
       <c r="D195">
         <v>5</v>
@@ -5000,10 +4946,10 @@
         <v>5</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D196">
         <v>5</v>
@@ -5014,10 +4960,10 @@
         <v>5</v>
       </c>
       <c r="B197" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="C197" s="3" t="s">
         <v>377</v>
-      </c>
-      <c r="C197" s="3" t="s">
-        <v>378</v>
       </c>
       <c r="D197">
         <v>5</v>
@@ -5028,10 +4974,10 @@
         <v>5</v>
       </c>
       <c r="B198" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="C198" s="3" t="s">
         <v>379</v>
-      </c>
-      <c r="C198" s="3" t="s">
-        <v>380</v>
       </c>
       <c r="D198">
         <v>5</v>
@@ -5042,10 +4988,10 @@
         <v>5</v>
       </c>
       <c r="B199" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="C199" s="3" t="s">
         <v>381</v>
-      </c>
-      <c r="C199" s="3" t="s">
-        <v>382</v>
       </c>
       <c r="D199">
         <v>5</v>
@@ -5056,10 +5002,10 @@
         <v>5</v>
       </c>
       <c r="B200" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="C200" s="3" t="s">
         <v>383</v>
-      </c>
-      <c r="C200" s="3" t="s">
-        <v>384</v>
       </c>
       <c r="D200">
         <v>5</v>
@@ -5070,10 +5016,10 @@
         <v>5</v>
       </c>
       <c r="B201" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="C201" s="3" t="s">
         <v>385</v>
-      </c>
-      <c r="C201" s="3" t="s">
-        <v>386</v>
       </c>
       <c r="D201">
         <v>5</v>
@@ -5084,10 +5030,10 @@
         <v>5</v>
       </c>
       <c r="B202" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="C202" s="3" t="s">
         <v>387</v>
-      </c>
-      <c r="C202" s="3" t="s">
-        <v>388</v>
       </c>
       <c r="D202">
         <v>5</v>
@@ -5098,10 +5044,10 @@
         <v>5</v>
       </c>
       <c r="B203" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C203" s="3" t="s">
         <v>389</v>
-      </c>
-      <c r="C203" s="3" t="s">
-        <v>390</v>
       </c>
       <c r="D203">
         <v>5</v>
@@ -5112,10 +5058,10 @@
         <v>5</v>
       </c>
       <c r="B204" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="C204" s="3" t="s">
         <v>391</v>
-      </c>
-      <c r="C204" s="3" t="s">
-        <v>392</v>
       </c>
       <c r="D204">
         <v>5</v>
@@ -5126,10 +5072,10 @@
         <v>5</v>
       </c>
       <c r="B205" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="C205" s="3" t="s">
         <v>393</v>
-      </c>
-      <c r="C205" s="3" t="s">
-        <v>394</v>
       </c>
       <c r="D205">
         <v>5</v>
@@ -5140,10 +5086,10 @@
         <v>5</v>
       </c>
       <c r="B206" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="C206" s="3" t="s">
         <v>395</v>
-      </c>
-      <c r="C206" s="3" t="s">
-        <v>396</v>
       </c>
       <c r="D206">
         <v>5</v>
@@ -5154,10 +5100,10 @@
         <v>5</v>
       </c>
       <c r="B207" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="C207" s="3" t="s">
         <v>397</v>
-      </c>
-      <c r="C207" s="3" t="s">
-        <v>398</v>
       </c>
       <c r="D207">
         <v>5</v>
@@ -5168,10 +5114,10 @@
         <v>5</v>
       </c>
       <c r="B208" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="C208" s="3" t="s">
         <v>399</v>
-      </c>
-      <c r="C208" s="3" t="s">
-        <v>400</v>
       </c>
       <c r="D208">
         <v>5</v>
@@ -5182,10 +5128,10 @@
         <v>5</v>
       </c>
       <c r="B209" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="C209" s="3" t="s">
         <v>401</v>
-      </c>
-      <c r="C209" s="3" t="s">
-        <v>402</v>
       </c>
       <c r="D209">
         <v>5</v>
@@ -5196,10 +5142,10 @@
         <v>5</v>
       </c>
       <c r="B210" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="C210" s="3" t="s">
         <v>403</v>
-      </c>
-      <c r="C210" s="3" t="s">
-        <v>404</v>
       </c>
       <c r="D210">
         <v>5</v>
@@ -5210,10 +5156,10 @@
         <v>5</v>
       </c>
       <c r="B211" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="C211" s="3" t="s">
         <v>405</v>
-      </c>
-      <c r="C211" s="3" t="s">
-        <v>406</v>
       </c>
       <c r="D211">
         <v>5</v>
@@ -5224,10 +5170,10 @@
         <v>5</v>
       </c>
       <c r="B212" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="C212" s="3" t="s">
         <v>407</v>
-      </c>
-      <c r="C212" s="3" t="s">
-        <v>408</v>
       </c>
       <c r="D212">
         <v>5</v>
@@ -5238,10 +5184,10 @@
         <v>5</v>
       </c>
       <c r="B213" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="C213" s="3" t="s">
         <v>409</v>
-      </c>
-      <c r="C213" s="3" t="s">
-        <v>410</v>
       </c>
       <c r="D213">
         <v>5</v>
@@ -5252,10 +5198,10 @@
         <v>5</v>
       </c>
       <c r="B214" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="C214" s="3" t="s">
         <v>411</v>
-      </c>
-      <c r="C214" s="3" t="s">
-        <v>412</v>
       </c>
       <c r="D214">
         <v>5</v>
@@ -5266,10 +5212,10 @@
         <v>5</v>
       </c>
       <c r="B215" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="C215" s="3" t="s">
         <v>413</v>
-      </c>
-      <c r="C215" s="3" t="s">
-        <v>414</v>
       </c>
       <c r="D215">
         <v>5</v>
@@ -5280,10 +5226,10 @@
         <v>5</v>
       </c>
       <c r="B216" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="C216" s="3" t="s">
         <v>415</v>
-      </c>
-      <c r="C216" s="3" t="s">
-        <v>416</v>
       </c>
       <c r="D216">
         <v>5</v>
@@ -5294,10 +5240,10 @@
         <v>5</v>
       </c>
       <c r="B217" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="C217" s="3" t="s">
         <v>417</v>
-      </c>
-      <c r="C217" s="3" t="s">
-        <v>418</v>
       </c>
       <c r="D217">
         <v>5</v>
@@ -5308,10 +5254,10 @@
         <v>5</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C218" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D218">
         <v>5</v>
@@ -5322,10 +5268,10 @@
         <v>5</v>
       </c>
       <c r="B219" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="C219" s="3" t="s">
         <v>420</v>
-      </c>
-      <c r="C219" s="3" t="s">
-        <v>421</v>
       </c>
       <c r="D219">
         <v>5</v>
@@ -5336,10 +5282,10 @@
         <v>5</v>
       </c>
       <c r="B220" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="C220" s="3" t="s">
         <v>422</v>
-      </c>
-      <c r="C220" s="3" t="s">
-        <v>423</v>
       </c>
       <c r="D220">
         <v>5</v>
@@ -5350,10 +5296,10 @@
         <v>5</v>
       </c>
       <c r="B221" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="C221" s="3" t="s">
         <v>424</v>
-      </c>
-      <c r="C221" s="3" t="s">
-        <v>425</v>
       </c>
       <c r="D221">
         <v>5</v>
@@ -5364,10 +5310,10 @@
         <v>5</v>
       </c>
       <c r="B222" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="C222" s="3" t="s">
         <v>426</v>
-      </c>
-      <c r="C222" s="3" t="s">
-        <v>427</v>
       </c>
       <c r="D222">
         <v>5</v>
@@ -5378,10 +5324,10 @@
         <v>5</v>
       </c>
       <c r="B223" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="C223" s="3" t="s">
         <v>428</v>
-      </c>
-      <c r="C223" s="3" t="s">
-        <v>429</v>
       </c>
       <c r="D223">
         <v>5</v>
@@ -5392,10 +5338,10 @@
         <v>5</v>
       </c>
       <c r="B224" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="C224" s="3" t="s">
         <v>430</v>
-      </c>
-      <c r="C224" s="3" t="s">
-        <v>431</v>
       </c>
       <c r="D224">
         <v>5</v>
@@ -5406,17 +5352,24 @@
         <v>5</v>
       </c>
       <c r="B225" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="C225" s="3" t="s">
         <v>432</v>
       </c>
-      <c r="C225" s="3" t="s">
-        <v>433</v>
-      </c>
       <c r="D225">
         <v>5</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2"/>
+    <hyperlink ref="C9"/>
+  </hyperlinks>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>